<commit_message>
feat: excel report for drivers
</commit_message>
<xml_diff>
--- a/orders/excel_templates/daily_report.xlsx
+++ b/orders/excel_templates/daily_report.xlsx
@@ -133,12 +133,103 @@
         </r>
       </text>
     </comment>
+    <comment ref="U1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>Автор:
+000000400</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>Автор:
+000000402</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>Автор:
+000000401</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>Автор:
+000000404</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>Автор:
+000000406</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>Автор:
+000000405</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>Автор:
+000000403</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Заказчик</t>
   </si>
@@ -171,6 +262,27 @@
   </si>
   <si>
     <t>Рсос</t>
+  </si>
+  <si>
+    <t>Рпик</t>
+  </si>
+  <si>
+    <t>Б.кур</t>
+  </si>
+  <si>
+    <t>Б.вет</t>
+  </si>
+  <si>
+    <t>Б.рыб</t>
+  </si>
+  <si>
+    <t>Б.сгу</t>
+  </si>
+  <si>
+    <t>Б.тво</t>
+  </si>
+  <si>
+    <t>Б.дже</t>
   </si>
   <si>
     <t>Итого</t>
@@ -297,7 +409,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -313,31 +425,34 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -358,8 +473,8 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ffff0000"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1428,7 +1543,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1452,10 +1567,21 @@
     <col min="18" max="18" width="5.35156" style="1" customWidth="1"/>
     <col min="19" max="19" width="4.67188" style="1" customWidth="1"/>
     <col min="20" max="20" width="5.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="3" style="1" customWidth="1"/>
-    <col min="22" max="22" width="6" style="1" customWidth="1"/>
-    <col min="23" max="23" width="39.1719" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="21" max="21" width="4.67188" style="1" customWidth="1"/>
+    <col min="22" max="22" width="5.35156" style="1" customWidth="1"/>
+    <col min="23" max="23" width="4.67188" style="1" customWidth="1"/>
+    <col min="24" max="24" width="5.85156" style="1" customWidth="1"/>
+    <col min="25" max="27" width="4.67188" style="1" customWidth="1"/>
+    <col min="28" max="28" width="5.35156" style="1" customWidth="1"/>
+    <col min="29" max="29" width="4.67188" style="1" customWidth="1"/>
+    <col min="30" max="30" width="5.85156" style="1" customWidth="1"/>
+    <col min="31" max="31" width="4.67188" style="1" customWidth="1"/>
+    <col min="32" max="32" width="5.35156" style="1" customWidth="1"/>
+    <col min="33" max="33" width="4.67188" style="1" customWidth="1"/>
+    <col min="34" max="34" width="5.5" style="1" customWidth="1"/>
+    <col min="35" max="35" width="6" style="1" customWidth="1"/>
+    <col min="36" max="36" width="39.1719" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="33.6" customHeight="1">
@@ -1501,41 +1627,81 @@
         <v>10</v>
       </c>
       <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" t="s" s="2">
+      <c r="U1" t="s" s="5">
         <v>11</v>
       </c>
+      <c r="V1" s="6"/>
       <c r="W1" t="s" s="5">
         <v>12</v>
       </c>
+      <c r="X1" s="6"/>
+      <c r="Y1" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="6"/>
+      <c r="AA1" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="AB1" s="6"/>
+      <c r="AC1" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="AD1" s="6"/>
+      <c r="AE1" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="AF1" s="6"/>
+      <c r="AG1" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="AH1" s="6"/>
+      <c r="AI1" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="AJ1" t="s" s="7">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="13"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="16">
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="O1:P1"/>
@@ -1545,6 +1711,13 @@
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="25" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>